<commit_message>
Working code to find optimal parameters in long_term_output.py. Also updated the level designations in the DOE files
</commit_message>
<xml_diff>
--- a/DOE.xlsx
+++ b/DOE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/000bbfc4ba40a858/phd/Models/Production planning with historical weather data/Reactor-Dash-App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD15E80D-C462-403F-B83B-7AB568ADE93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2DF41B8-74B2-486D-BC69-F8EDF5055963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7D214A6-7DAF-4489-8D73-C889A1DFB1F9}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:F147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A108" sqref="A108:A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2555,7 +2555,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B110">
         <v>2</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B111">
         <v>2</v>
@@ -2635,7 +2635,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -2675,7 +2675,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B114">
         <v>2</v>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B115">
         <v>2</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B118">
         <v>2</v>
@@ -2775,7 +2775,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B119">
         <v>2</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -2815,7 +2815,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B122">
         <v>2</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B123">
         <v>2</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -2895,7 +2895,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2955,7 +2955,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2975,7 +2975,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -3075,7 +3075,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -3115,7 +3115,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -3135,7 +3135,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -3175,7 +3175,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -3215,7 +3215,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -3235,7 +3235,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -3295,7 +3295,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -3315,7 +3315,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -3335,7 +3335,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B147">
         <v>1</v>

</xml_diff>